<commit_message>
add randomized nodes in construction
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="GRASP (rec_enh_best_seed)" sheetId="5" r:id="rId1"/>
     <sheet name="GRASP (rec_enh_seed)" sheetId="1" r:id="rId2"/>
     <sheet name="GRASP (rec_seed)" sheetId="4" r:id="rId3"/>
+    <sheet name="GRASP (randnode_rec_seed)" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="11">
   <si>
     <t>Alpha\Instance</t>
   </si>
@@ -149,55 +150,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="41">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1421,57 +1374,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
       <formula>$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
       <formula>$D$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
       <formula>$E$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
       <formula>$H$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>$I$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>$J$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
       <formula>$K$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1926,52 +1879,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="cellIs" dxfId="44" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="10" operator="equal">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="43" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
       <formula>$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
       <formula>$D$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="41" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
       <formula>$E$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
       <formula>$H$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="37" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>$I$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>$J$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>$K$12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1987,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2426,52 +2379,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="cellIs" dxfId="34" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="33" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="32" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>$D$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="31" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>$E$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="29" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>$H$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>$I$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>$J$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>$K$12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2481,4 +2434,501 @@
     <ignoredError sqref="B1:K1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>42783759</v>
+      </c>
+      <c r="D2">
+        <v>133241309</v>
+      </c>
+      <c r="E2">
+        <v>7686</v>
+      </c>
+      <c r="F2">
+        <v>39144</v>
+      </c>
+      <c r="G2">
+        <v>22068</v>
+      </c>
+      <c r="H2">
+        <v>103247</v>
+      </c>
+      <c r="I2">
+        <v>95859</v>
+      </c>
+      <c r="J2">
+        <v>34316</v>
+      </c>
+      <c r="K2">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>42630715</v>
+      </c>
+      <c r="D3">
+        <v>132987802</v>
+      </c>
+      <c r="E3">
+        <v>7713</v>
+      </c>
+      <c r="F3">
+        <v>40124</v>
+      </c>
+      <c r="G3">
+        <v>22068</v>
+      </c>
+      <c r="H3">
+        <v>106706</v>
+      </c>
+      <c r="I3">
+        <v>94829</v>
+      </c>
+      <c r="J3">
+        <v>34316</v>
+      </c>
+      <c r="K3">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>42630715</v>
+      </c>
+      <c r="D4">
+        <v>132894610</v>
+      </c>
+      <c r="E4">
+        <v>7375</v>
+      </c>
+      <c r="F4">
+        <v>39274</v>
+      </c>
+      <c r="G4">
+        <v>22068</v>
+      </c>
+      <c r="H4">
+        <v>103674</v>
+      </c>
+      <c r="I4">
+        <v>95797</v>
+      </c>
+      <c r="J4">
+        <v>34316</v>
+      </c>
+      <c r="K4">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>42085075</v>
+      </c>
+      <c r="D5">
+        <v>132894610</v>
+      </c>
+      <c r="E5">
+        <v>7511</v>
+      </c>
+      <c r="F5">
+        <v>39274</v>
+      </c>
+      <c r="G5">
+        <v>22068</v>
+      </c>
+      <c r="H5">
+        <v>106562</v>
+      </c>
+      <c r="I5">
+        <v>98072</v>
+      </c>
+      <c r="J5">
+        <v>34316</v>
+      </c>
+      <c r="K5">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>42085075</v>
+      </c>
+      <c r="D6">
+        <v>132330304</v>
+      </c>
+      <c r="E6">
+        <v>7382</v>
+      </c>
+      <c r="F6">
+        <v>38304</v>
+      </c>
+      <c r="G6">
+        <v>22068</v>
+      </c>
+      <c r="H6">
+        <v>106151</v>
+      </c>
+      <c r="I6">
+        <v>102485</v>
+      </c>
+      <c r="J6">
+        <v>34316</v>
+      </c>
+      <c r="K6">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>42630715</v>
+      </c>
+      <c r="D7">
+        <v>131022310</v>
+      </c>
+      <c r="E7">
+        <v>7382</v>
+      </c>
+      <c r="F7">
+        <v>36628</v>
+      </c>
+      <c r="G7">
+        <v>22068</v>
+      </c>
+      <c r="H7">
+        <v>106937</v>
+      </c>
+      <c r="I7">
+        <v>101839</v>
+      </c>
+      <c r="J7">
+        <v>34316</v>
+      </c>
+      <c r="K7">
+        <v>80343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>42630715</v>
+      </c>
+      <c r="D8">
+        <v>130736205</v>
+      </c>
+      <c r="E8">
+        <v>7370</v>
+      </c>
+      <c r="F8">
+        <v>39214</v>
+      </c>
+      <c r="G8">
+        <v>22068</v>
+      </c>
+      <c r="H8">
+        <v>104879</v>
+      </c>
+      <c r="I8">
+        <v>102892</v>
+      </c>
+      <c r="J8">
+        <v>34316</v>
+      </c>
+      <c r="K8">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>42661819</v>
+      </c>
+      <c r="D9">
+        <v>131719633</v>
+      </c>
+      <c r="E9">
+        <v>7425</v>
+      </c>
+      <c r="F9">
+        <v>40264</v>
+      </c>
+      <c r="G9">
+        <v>22068</v>
+      </c>
+      <c r="H9">
+        <v>108186</v>
+      </c>
+      <c r="I9">
+        <v>102892</v>
+      </c>
+      <c r="J9">
+        <v>34316</v>
+      </c>
+      <c r="K9">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>42630715</v>
+      </c>
+      <c r="D10">
+        <v>131022310</v>
+      </c>
+      <c r="E10">
+        <v>7586</v>
+      </c>
+      <c r="F10">
+        <v>39314</v>
+      </c>
+      <c r="G10">
+        <v>22068</v>
+      </c>
+      <c r="H10">
+        <v>109672</v>
+      </c>
+      <c r="I10">
+        <v>102892</v>
+      </c>
+      <c r="J10">
+        <v>34316</v>
+      </c>
+      <c r="K10">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5">
+        <v>42783759</v>
+      </c>
+      <c r="D11" s="5">
+        <v>131022310</v>
+      </c>
+      <c r="E11" s="5">
+        <v>7568</v>
+      </c>
+      <c r="F11" s="5">
+        <v>42164</v>
+      </c>
+      <c r="G11" s="5">
+        <v>22068</v>
+      </c>
+      <c r="H11" s="5">
+        <v>102892</v>
+      </c>
+      <c r="I11" s="5">
+        <v>102892</v>
+      </c>
+      <c r="J11">
+        <v>34316</v>
+      </c>
+      <c r="K11">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1"/>
+      <c r="B12">
+        <f>MIN(B2:B11)</f>
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:K12" si="0">MIN(C2:C11)</f>
+        <v>42085075</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>130736205</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>7370</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>36628</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>22068</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>102892</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>94829</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="0"/>
+        <v>34316</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="0"/>
+        <v>80343</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B11">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>$B$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C11">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>$C$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D11">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>$D$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E11">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>$E$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F11">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>$F$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G11">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>$G$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H11">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>$H$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I11">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>$I$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J11">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>$J$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K11">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>$K$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bugfix in steiner tree rebuilding alternative random node including tests (commented out for now) run_opt script
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GRASP (rec_enh_best_seed)" sheetId="5" r:id="rId1"/>
     <sheet name="GRASP (rec_enh_seed)" sheetId="1" r:id="rId2"/>
     <sheet name="GRASP (rec_seed)" sheetId="4" r:id="rId3"/>
     <sheet name="GRASP (randnode_rec_seed)" sheetId="6" r:id="rId4"/>
+    <sheet name="GRASP (randnode2_rec_seed)" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="11">
   <si>
     <t>Alpha\Instance</t>
   </si>
@@ -150,7 +151,139 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="52">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1374,57 +1507,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="11" operator="equal">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="10" operator="equal">
       <formula>$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="9" operator="equal">
       <formula>$D$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="8" operator="equal">
       <formula>$E$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="7" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="6" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
       <formula>$H$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
       <formula>$I$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
       <formula>$J$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>$K$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1879,52 +2012,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="cellIs" dxfId="29" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="10" operator="equal">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
       <formula>$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="27" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
       <formula>$D$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="7" operator="equal">
       <formula>$E$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
       <formula>$H$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>$I$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>$J$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>$K$12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2379,52 +2512,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="9" operator="equal">
       <formula>$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
       <formula>$D$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
       <formula>$E$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>$H$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>$I$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>$J$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>$K$12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2440,8 +2573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2822,7 +2955,7 @@
         <v>22068</v>
       </c>
       <c r="H11" s="5">
-        <v>102892</v>
+        <v>109672</v>
       </c>
       <c r="I11" s="5">
         <v>102892</v>
@@ -2862,7 +2995,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="0"/>
-        <v>102892</v>
+        <v>103247</v>
       </c>
       <c r="I12">
         <f t="shared" si="0"/>
@@ -2879,56 +3012,553 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
       <formula>$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
       <formula>$D$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
       <formula>$E$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>$H$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>$I$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>$J$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>$K$12</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>42783759</v>
+      </c>
+      <c r="D2">
+        <v>132894610</v>
+      </c>
+      <c r="E2">
+        <v>7616</v>
+      </c>
+      <c r="F2">
+        <v>39144</v>
+      </c>
+      <c r="G2">
+        <v>22068</v>
+      </c>
+      <c r="H2">
+        <v>102794</v>
+      </c>
+      <c r="I2">
+        <v>95859</v>
+      </c>
+      <c r="J2">
+        <v>34316</v>
+      </c>
+      <c r="K2">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>42783759</v>
+      </c>
+      <c r="D3">
+        <v>132987802</v>
+      </c>
+      <c r="E3">
+        <v>7375</v>
+      </c>
+      <c r="F3">
+        <v>39254</v>
+      </c>
+      <c r="G3">
+        <v>22068</v>
+      </c>
+      <c r="H3">
+        <v>105772</v>
+      </c>
+      <c r="I3">
+        <v>96026</v>
+      </c>
+      <c r="J3">
+        <v>34316</v>
+      </c>
+      <c r="K3">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>42630715</v>
+      </c>
+      <c r="D4">
+        <v>132894610</v>
+      </c>
+      <c r="E4">
+        <v>7375</v>
+      </c>
+      <c r="F4">
+        <v>38561</v>
+      </c>
+      <c r="G4">
+        <v>22068</v>
+      </c>
+      <c r="H4">
+        <v>106214</v>
+      </c>
+      <c r="I4">
+        <v>95781</v>
+      </c>
+      <c r="J4">
+        <v>34316</v>
+      </c>
+      <c r="K4">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>42085075</v>
+      </c>
+      <c r="D5">
+        <v>132894610</v>
+      </c>
+      <c r="E5">
+        <v>7407</v>
+      </c>
+      <c r="F5">
+        <v>38826</v>
+      </c>
+      <c r="G5">
+        <v>22068</v>
+      </c>
+      <c r="H5">
+        <v>107208</v>
+      </c>
+      <c r="I5">
+        <v>97304</v>
+      </c>
+      <c r="J5">
+        <v>34316</v>
+      </c>
+      <c r="K5">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>42630715</v>
+      </c>
+      <c r="D6">
+        <v>132330304</v>
+      </c>
+      <c r="E6">
+        <v>7382</v>
+      </c>
+      <c r="F6">
+        <v>38485</v>
+      </c>
+      <c r="G6">
+        <v>22068</v>
+      </c>
+      <c r="H6">
+        <v>108199</v>
+      </c>
+      <c r="I6">
+        <v>102892</v>
+      </c>
+      <c r="J6">
+        <v>34316</v>
+      </c>
+      <c r="K6">
+        <v>80236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>42630715</v>
+      </c>
+      <c r="D7">
+        <v>132245121</v>
+      </c>
+      <c r="E7">
+        <v>7610</v>
+      </c>
+      <c r="F7">
+        <v>38334</v>
+      </c>
+      <c r="G7">
+        <v>22068</v>
+      </c>
+      <c r="H7">
+        <v>108760</v>
+      </c>
+      <c r="I7">
+        <v>102005</v>
+      </c>
+      <c r="J7">
+        <v>34316</v>
+      </c>
+      <c r="K7">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>42630715</v>
+      </c>
+      <c r="D8">
+        <v>132245121</v>
+      </c>
+      <c r="E8">
+        <v>7610</v>
+      </c>
+      <c r="F8">
+        <v>38334</v>
+      </c>
+      <c r="G8">
+        <v>22068</v>
+      </c>
+      <c r="H8">
+        <v>108760</v>
+      </c>
+      <c r="I8">
+        <v>102005</v>
+      </c>
+      <c r="J8">
+        <v>34316</v>
+      </c>
+      <c r="K8">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>42447877</v>
+      </c>
+      <c r="D9">
+        <v>131294566</v>
+      </c>
+      <c r="E9">
+        <v>7307</v>
+      </c>
+      <c r="F9">
+        <v>40154</v>
+      </c>
+      <c r="G9">
+        <v>22068</v>
+      </c>
+      <c r="H9">
+        <v>106314</v>
+      </c>
+      <c r="I9">
+        <v>102892</v>
+      </c>
+      <c r="J9">
+        <v>34316</v>
+      </c>
+      <c r="K9">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>42630715</v>
+      </c>
+      <c r="D10">
+        <v>131294566</v>
+      </c>
+      <c r="E10">
+        <v>7503</v>
+      </c>
+      <c r="F10">
+        <v>40234</v>
+      </c>
+      <c r="G10">
+        <v>22068</v>
+      </c>
+      <c r="H10">
+        <v>108986</v>
+      </c>
+      <c r="I10">
+        <v>102892</v>
+      </c>
+      <c r="J10">
+        <v>34316</v>
+      </c>
+      <c r="K10">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5">
+        <v>42783759</v>
+      </c>
+      <c r="D11" s="5">
+        <v>131022310</v>
+      </c>
+      <c r="E11" s="5">
+        <v>7434</v>
+      </c>
+      <c r="F11" s="5">
+        <v>42204</v>
+      </c>
+      <c r="G11" s="5">
+        <v>22068</v>
+      </c>
+      <c r="H11" s="5">
+        <v>107522</v>
+      </c>
+      <c r="I11" s="5">
+        <v>102892</v>
+      </c>
+      <c r="J11">
+        <v>34316</v>
+      </c>
+      <c r="K11">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1"/>
+      <c r="B12">
+        <f>MIN(B2:B11)</f>
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:K12" si="0">MIN(C2:C11)</f>
+        <v>42085075</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>131022310</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>7307</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>38334</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>22068</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>102794</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>95781</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="0"/>
+        <v>34316</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="0"/>
+        <v>80236</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B11">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>$B$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C11">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>$C$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D11">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>$D$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E11">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>$E$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F11">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>$F$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G11">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>$G$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H11">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>$H$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I11">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>$I$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J11">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>$J$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K11">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>$K$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
evaluation of fixed results
</commit_message>
<xml_diff>
--- a/evaluation.xlsx
+++ b/evaluation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="GRASP (rec_enh_best_seed)" sheetId="5" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="GRASP (rec_seed)" sheetId="4" r:id="rId3"/>
     <sheet name="GRASP (randnode_rec_seed)" sheetId="6" r:id="rId4"/>
     <sheet name="GRASP (randnode2_rec_seed)" sheetId="7" r:id="rId5"/>
+    <sheet name="GRASP (randnode_rec_seed) FIXED" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="11">
   <si>
     <t>Alpha\Instance</t>
   </si>
@@ -151,7 +152,127 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="62">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1507,57 +1628,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="cellIs" dxfId="51" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="11" operator="equal">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="50" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="10" operator="equal">
       <formula>$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="49" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
       <formula>$D$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="48" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="8" operator="equal">
       <formula>$E$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="cellIs" dxfId="47" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="7" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="46" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="6" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="5" operator="equal">
       <formula>$H$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="4" operator="equal">
       <formula>$I$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
       <formula>$J$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="2" operator="equal">
       <formula>$K$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="1" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2012,52 +2133,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="cellIs" dxfId="40" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="10" operator="equal">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="9" operator="equal">
       <formula>$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="8" operator="equal">
       <formula>$D$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="37" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="7" operator="equal">
       <formula>$E$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="6" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
       <formula>$H$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
       <formula>$I$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>$J$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>$K$12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2512,52 +2633,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="10" operator="equal">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="29" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
       <formula>$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
       <formula>$D$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="7" operator="equal">
       <formula>$E$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
       <formula>$H$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>$I$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>$J$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>$K$12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2574,7 +2695,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3012,52 +3133,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
       <formula>$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="9" operator="equal">
       <formula>$C$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D11">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
       <formula>$D$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E11">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
       <formula>$E$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F11">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
       <formula>$F$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
       <formula>$G$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>$H$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I11">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>$I$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J11">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>$J$12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K11">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>$K$12</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3070,7 +3191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -3509,6 +3630,503 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B11">
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+      <formula>$B$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C11">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+      <formula>$C$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D11">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+      <formula>$D$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E11">
+    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+      <formula>$E$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F11">
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+      <formula>$F$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G11">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+      <formula>$G$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H11">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+      <formula>$H$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I11">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+      <formula>$I$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J11">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+      <formula>$J$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K11">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>$K$12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>42783759</v>
+      </c>
+      <c r="D2">
+        <v>133241309</v>
+      </c>
+      <c r="E2">
+        <v>7616</v>
+      </c>
+      <c r="F2">
+        <v>39144</v>
+      </c>
+      <c r="G2">
+        <v>22068</v>
+      </c>
+      <c r="H2">
+        <v>102617</v>
+      </c>
+      <c r="I2">
+        <v>95859</v>
+      </c>
+      <c r="J2">
+        <v>34316</v>
+      </c>
+      <c r="K2">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>42630715</v>
+      </c>
+      <c r="D3">
+        <v>132987802</v>
+      </c>
+      <c r="E3">
+        <v>7713</v>
+      </c>
+      <c r="F3">
+        <v>40124</v>
+      </c>
+      <c r="G3">
+        <v>22068</v>
+      </c>
+      <c r="H3">
+        <v>105876</v>
+      </c>
+      <c r="I3">
+        <v>94829</v>
+      </c>
+      <c r="J3">
+        <v>34316</v>
+      </c>
+      <c r="K3">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>42630715</v>
+      </c>
+      <c r="D4">
+        <v>131957632</v>
+      </c>
+      <c r="E4">
+        <v>7375</v>
+      </c>
+      <c r="F4">
+        <v>39274</v>
+      </c>
+      <c r="G4">
+        <v>22068</v>
+      </c>
+      <c r="H4">
+        <v>102750</v>
+      </c>
+      <c r="I4">
+        <v>96617</v>
+      </c>
+      <c r="J4">
+        <v>34316</v>
+      </c>
+      <c r="K4">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>42085075</v>
+      </c>
+      <c r="D5">
+        <v>132894610</v>
+      </c>
+      <c r="E5">
+        <v>7511</v>
+      </c>
+      <c r="F5">
+        <v>39274</v>
+      </c>
+      <c r="G5">
+        <v>22068</v>
+      </c>
+      <c r="H5">
+        <v>106562</v>
+      </c>
+      <c r="I5">
+        <v>98072</v>
+      </c>
+      <c r="J5">
+        <v>34316</v>
+      </c>
+      <c r="K5">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>42085075</v>
+      </c>
+      <c r="D6">
+        <v>132330304</v>
+      </c>
+      <c r="E6">
+        <v>7549</v>
+      </c>
+      <c r="F6">
+        <v>38304</v>
+      </c>
+      <c r="G6">
+        <v>22068</v>
+      </c>
+      <c r="H6">
+        <v>106151</v>
+      </c>
+      <c r="I6">
+        <v>102485</v>
+      </c>
+      <c r="J6">
+        <v>34316</v>
+      </c>
+      <c r="K6">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>42630715</v>
+      </c>
+      <c r="D7">
+        <v>131022310</v>
+      </c>
+      <c r="E7">
+        <v>7382</v>
+      </c>
+      <c r="F7">
+        <v>36628</v>
+      </c>
+      <c r="G7">
+        <v>22068</v>
+      </c>
+      <c r="H7">
+        <v>106129</v>
+      </c>
+      <c r="I7">
+        <v>101839</v>
+      </c>
+      <c r="J7">
+        <v>34316</v>
+      </c>
+      <c r="K7">
+        <v>80343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>42630715</v>
+      </c>
+      <c r="D8">
+        <v>130736205</v>
+      </c>
+      <c r="E8">
+        <v>7370</v>
+      </c>
+      <c r="F8">
+        <v>39214</v>
+      </c>
+      <c r="G8">
+        <v>22068</v>
+      </c>
+      <c r="H8">
+        <v>104879</v>
+      </c>
+      <c r="I8">
+        <v>103455</v>
+      </c>
+      <c r="J8">
+        <v>34316</v>
+      </c>
+      <c r="K8">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>42661819</v>
+      </c>
+      <c r="D9">
+        <v>131719633</v>
+      </c>
+      <c r="E9">
+        <v>7425</v>
+      </c>
+      <c r="F9">
+        <v>40264</v>
+      </c>
+      <c r="G9">
+        <v>22068</v>
+      </c>
+      <c r="H9">
+        <v>107586</v>
+      </c>
+      <c r="I9">
+        <v>103455</v>
+      </c>
+      <c r="J9">
+        <v>34316</v>
+      </c>
+      <c r="K9">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>42630715</v>
+      </c>
+      <c r="D10">
+        <v>131022310</v>
+      </c>
+      <c r="E10">
+        <v>7586</v>
+      </c>
+      <c r="F10">
+        <v>39314</v>
+      </c>
+      <c r="G10">
+        <v>22068</v>
+      </c>
+      <c r="H10">
+        <v>109381</v>
+      </c>
+      <c r="I10">
+        <v>103455</v>
+      </c>
+      <c r="J10">
+        <v>34316</v>
+      </c>
+      <c r="K10">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5">
+        <v>42783759</v>
+      </c>
+      <c r="D11" s="5">
+        <v>131022310</v>
+      </c>
+      <c r="E11" s="5">
+        <v>7568</v>
+      </c>
+      <c r="F11" s="5">
+        <v>42164</v>
+      </c>
+      <c r="G11" s="5">
+        <v>22068</v>
+      </c>
+      <c r="H11" s="5">
+        <v>109326</v>
+      </c>
+      <c r="I11" s="5">
+        <v>103455</v>
+      </c>
+      <c r="J11">
+        <v>34316</v>
+      </c>
+      <c r="K11">
+        <v>80775</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="1"/>
+      <c r="B12">
+        <f>MIN(B2:B11)</f>
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:K12" si="0">MIN(C2:C11)</f>
+        <v>42085075</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>130736205</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>7370</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>36628</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>22068</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>102617</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>94829</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="0"/>
+        <v>34316</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="0"/>
+        <v>80343</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B11">
     <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>$B$12</formula>
     </cfRule>

</xml_diff>